<commit_message>
Add example usage scripts and comprehensive tests for API functionality
- Created `ejemplos_uso.py` to demonstrate various API functionalities including simple queries, concurrent downloads, and handling multiple formats.
- Added `test_actualizacion.py` to verify imports, function signatures, request structures, and API endpoints.
- Implemented `test_api_response.py` to check the API response and validate MinIO fields.
- Developed `test_descarga_real.py` to simulate the complete download process, including CSV reading, directory creation, and file extraction.
</commit_message>
<xml_diff>
--- a/Descarga-Mis-Comprobantes.xlsx
+++ b/Descarga-Mis-Comprobantes.xlsx
@@ -49,13 +49,13 @@
     <t xml:space="preserve">Descarga Recibidos</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubicación Emitidos</t>
+    <t xml:space="preserve">Ubicacion Emitidos</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Emitidos</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubicación Recibidos</t>
+    <t xml:space="preserve">Ubicacion Recibidos</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Recibidos</t>
@@ -375,7 +375,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>